<commit_message>
Add analysis for P1 excel file
</commit_message>
<xml_diff>
--- a/analysisP1.xlsx
+++ b/analysisP1.xlsx
@@ -24,45 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Bias</t>
-  </si>
-  <si>
-    <t>BagSize1, TreeSize1</t>
-  </si>
-  <si>
-    <t>BagSize1, TreeSize2</t>
-  </si>
-  <si>
-    <t>BagSize1, TreeSize3</t>
-  </si>
-  <si>
-    <t>BagSize2, TreeSize1</t>
-  </si>
-  <si>
-    <t>BagSize2, TreeSize2</t>
-  </si>
-  <si>
-    <t>BagSize2, TreeSize3</t>
-  </si>
-  <si>
-    <t>BagSize5, TreeSize1</t>
-  </si>
-  <si>
-    <t>BagSize5, TreeSize2</t>
-  </si>
-  <si>
-    <t>BagSize5, TreeSize3</t>
-  </si>
-  <si>
-    <t>BagSize10, TreeSize1</t>
-  </si>
-  <si>
-    <t>BagSize10, TreeSize2</t>
-  </si>
-  <si>
-    <t>BagSize10, TreeSize3</t>
   </si>
   <si>
     <t>Configuration</t>
@@ -70,14 +34,66 @@
   <si>
     <t>Variance2</t>
   </si>
+  <si>
+    <t>BagSize1, TreeDepth1</t>
+  </si>
+  <si>
+    <t>BagSize1, TreeDepth2</t>
+  </si>
+  <si>
+    <t>BagSize1, TreeDepth3</t>
+  </si>
+  <si>
+    <t>BagSize2, TreeDepth1</t>
+  </si>
+  <si>
+    <t>BagSize2, TreeDepth2</t>
+  </si>
+  <si>
+    <t>BagSize2, TreeDepth3</t>
+  </si>
+  <si>
+    <t>BagSize5, TreeDepth1</t>
+  </si>
+  <si>
+    <t>BagSize5, TreeDepth2</t>
+  </si>
+  <si>
+    <t>BagSize5, TreeDepth3</t>
+  </si>
+  <si>
+    <t>BagSize10, TreeDepth1</t>
+  </si>
+  <si>
+    <t>BagSize10, TreeDepth2</t>
+  </si>
+  <si>
+    <t>BagSize10, TreeDepth3</t>
+  </si>
+  <si>
+    <t>AccuracyTraining</t>
+  </si>
+  <si>
+    <t>AccuracyTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -104,13 +120,119 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -274,40 +396,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>BagSize1, TreeSize1</c:v>
+                  <c:v>BagSize1, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BagSize1, TreeSize2</c:v>
+                  <c:v>BagSize1, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BagSize1, TreeSize3</c:v>
+                  <c:v>BagSize1, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>BagSize2, TreeSize1</c:v>
+                  <c:v>BagSize2, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>BagSize2, TreeSize2</c:v>
+                  <c:v>BagSize2, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BagSize2, TreeSize3</c:v>
+                  <c:v>BagSize2, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>BagSize5, TreeSize1</c:v>
+                  <c:v>BagSize5, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>BagSize5, TreeSize2</c:v>
+                  <c:v>BagSize5, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>BagSize5, TreeSize3</c:v>
+                  <c:v>BagSize5, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>BagSize10, TreeSize1</c:v>
+                  <c:v>BagSize10, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>BagSize10, TreeSize2</c:v>
+                  <c:v>BagSize10, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>BagSize10, TreeSize3</c:v>
+                  <c:v>BagSize10, TreeDepth3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -316,7 +438,7 @@
             <c:numRef>
               <c:f>Sheet1!$G$3:$G$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.18198662309368199</c:v>
@@ -457,7 +579,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -750,40 +872,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>BagSize1, TreeSize1</c:v>
+                  <c:v>BagSize1, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BagSize1, TreeSize2</c:v>
+                  <c:v>BagSize1, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BagSize1, TreeSize3</c:v>
+                  <c:v>BagSize1, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>BagSize2, TreeSize1</c:v>
+                  <c:v>BagSize2, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>BagSize2, TreeSize2</c:v>
+                  <c:v>BagSize2, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BagSize2, TreeSize3</c:v>
+                  <c:v>BagSize2, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>BagSize5, TreeSize1</c:v>
+                  <c:v>BagSize5, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>BagSize5, TreeSize2</c:v>
+                  <c:v>BagSize5, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>BagSize5, TreeSize3</c:v>
+                  <c:v>BagSize5, TreeDepth3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>BagSize10, TreeSize1</c:v>
+                  <c:v>BagSize10, TreeDepth1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>BagSize10, TreeSize2</c:v>
+                  <c:v>BagSize10, TreeDepth2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>BagSize10, TreeSize3</c:v>
+                  <c:v>BagSize10, TreeDepth3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -792,7 +914,7 @@
             <c:numRef>
               <c:f>Sheet1!$H$3:$H$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>7.7516339869281004E-4</c:v>
@@ -933,7 +1055,969 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="295881464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> against training data</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AccuracyTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$F$3:$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>BagSize1, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BagSize1, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BagSize1, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BagSize2, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BagSize2, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BagSize2, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BagSize5, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BagSize5, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>BagSize5, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BagSize10, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>BagSize10, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>BagSize10, TreeDepth3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.81757124183006502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81916732026143801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82178169934640499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81756339869281103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81893594771241895</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82261568627450998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81760130718954205</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82013594771241805</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.825664052287582</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81761045751633998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82013071895424805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82643137254901999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4222-41A3-BF25-33C8E3588136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="295881464"/>
+        <c:axId val="296928760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="295881464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296928760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296928760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="295881464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> against test data</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AccuracyTest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$F$3:$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>BagSize1, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BagSize1, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BagSize1, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BagSize2, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BagSize2, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BagSize2, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BagSize5, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BagSize5, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>BagSize5, TreeDepth3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BagSize10, TreeDepth1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>BagSize10, TreeDepth2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>BagSize10, TreeDepth3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.83065185185185197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83025185185185202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82656296296296305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83057037037036996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82916296296296299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82568888888888903</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83070370370370405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83122222222222197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83117777777777802</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83065185185185197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83071111111111096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83122962962962998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-70B5-43DA-9DAE-0B17CCBFFE37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="295881464"/>
+        <c:axId val="296928760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="295881464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296928760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296928760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1130,6 +2214,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2162,20 +3326,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2238,16 +4434,94 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB31B822-BC6A-4E91-B78F-F0F7E0139AA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CFA1192-3B4B-4E24-9165-CDA5BE0A004A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="F2:H14" totalsRowShown="0">
-  <autoFilter ref="F2:H14"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Configuration"/>
-    <tableColumn id="2" name="Bias"/>
-    <tableColumn id="4" name="Variance2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="F2:J14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="F2:J14"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Configuration" dataDxfId="4"/>
+    <tableColumn id="2" name="Bias" dataDxfId="3"/>
+    <tableColumn id="4" name="Variance2" dataDxfId="2"/>
+    <tableColumn id="5" name="AccuracyTraining" dataDxfId="1"/>
+    <tableColumn id="6" name="AccuracyTest" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2550,165 +4824,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F2:H14"/>
+  <dimension ref="F2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.18198662309368199</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7.7516339869281004E-4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.81757124183006502</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.83065185185185197</v>
+      </c>
+    </row>
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.17209211328976001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.00209150326796E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.81916732026143801</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.83025185185185202</v>
+      </c>
+    </row>
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.16103294117647199</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.4132026143791299E-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.82178169934640499</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.82656296296296305</v>
+      </c>
+    </row>
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.182018997821351</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6.0653594771241804E-4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.81756339869281103</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.83057037037036996</v>
+      </c>
+    </row>
+    <row r="7" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.17547498910675399</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8.4300653594770406E-3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.81893594771241895</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.82916296296296299</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.16534501089324599</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.67424836601309E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.82261568627450998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.82568888888888903</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.182084183006536</v>
+      </c>
+      <c r="H9" s="2">
+        <v>6.4836601307189604E-4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.81760130718954205</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.83070370370370405</v>
+      </c>
+    </row>
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.174859825708061</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.3006535947712199E-3</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.82013594771241805</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.83122222222222197</v>
+      </c>
+    </row>
+    <row r="11" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.16616082788671099</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.27398692810458E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.825664052287582</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.83117777777777802</v>
+      </c>
+    </row>
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.18211403050108901</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.29411764705882E-4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.81761045751633998</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.83065185185185197</v>
+      </c>
+    </row>
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G13" s="2">
+        <v>0.178094989106754</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4.1973856209149996E-3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.82013071895424805</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.83071111111111096</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0.18198662309368199</v>
-      </c>
-      <c r="H3">
-        <v>7.7516339869281004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0.17209211328976001</v>
-      </c>
-      <c r="H4">
-        <v>1.00209150326796E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>0.16103294117647199</v>
-      </c>
-      <c r="H5">
-        <v>2.4132026143791299E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>0.182018997821351</v>
-      </c>
-      <c r="H6">
-        <v>6.0653594771241804E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>0.17547498910675399</v>
-      </c>
-      <c r="H7">
-        <v>8.4300653594770406E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <v>0.16534501089324599</v>
-      </c>
-      <c r="H8">
-        <v>1.67424836601309E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>0.182084183006536</v>
-      </c>
-      <c r="H9">
-        <v>6.4836601307189604E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>0.174859825708061</v>
-      </c>
-      <c r="H10">
-        <v>6.3006535947712199E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>0.16616082788671099</v>
-      </c>
-      <c r="H11">
-        <v>1.27398692810458E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>0.18211403050108901</v>
-      </c>
-      <c r="H12">
-        <v>3.29411764705882E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>0.178094989106754</v>
-      </c>
-      <c r="H13">
-        <v>4.1973856209149996E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>0.16800753812636199</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>7.7738562091503099E-3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.82643137254901999</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.83122962962962998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update analysis for P1
</commit_message>
<xml_diff>
--- a/analysisP1.xlsx
+++ b/analysisP1.xlsx
@@ -82,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -123,8 +123,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,7 +143,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -158,7 +158,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -173,7 +173,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -188,7 +188,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -4827,7 +4827,7 @@
   <dimension ref="F2:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection activeCell="F2" sqref="F2:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>